<commit_message>
Lagt til shunt admittanser.
</commit_message>
<xml_diff>
--- a/linjeimpedanser.xlsx
+++ b/linjeimpedanser.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arntzen/Desktop/IELET2118---Prosjekt-Lastflytanalyse/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F82FEC1-F8AB-6C4C-A3AF-972333F8C9C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6D1E4D4-9E93-714A-91B4-64814E64DE3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
   <si>
     <t>Linje</t>
   </si>
@@ -37,6 +37,15 @@
     <t>Kapasitans (nF)</t>
   </si>
   <si>
+    <t>Shunt Admittans (ohm)</t>
+  </si>
+  <si>
+    <t>Shunt Admittans (p.u.)</t>
+  </si>
+  <si>
+    <t>Shunt Admittans (p.u.) half</t>
+  </si>
+  <si>
     <t>1-2</t>
   </si>
   <si>
@@ -49,6 +58,15 @@
     <t>(0.8429-9.0614j)</t>
   </si>
   <si>
+    <t>62589.9504j</t>
+  </si>
+  <si>
+    <t>695.4439j</t>
+  </si>
+  <si>
+    <t>347.7219j</t>
+  </si>
+  <si>
     <t>2-3</t>
   </si>
   <si>
@@ -61,6 +79,15 @@
     <t>(1.0268-11.0376j)</t>
   </si>
   <si>
+    <t>51383.8894j</t>
+  </si>
+  <si>
+    <t>570.9321j</t>
+  </si>
+  <si>
+    <t>285.4661j</t>
+  </si>
+  <si>
     <t>3-4</t>
   </si>
   <si>
@@ -73,6 +100,15 @@
     <t>(0.4038-4.3411j)</t>
   </si>
   <si>
+    <t>130646.2721j</t>
+  </si>
+  <si>
+    <t>1451.6252j</t>
+  </si>
+  <si>
+    <t>725.8126j</t>
+  </si>
+  <si>
     <t>4-5</t>
   </si>
   <si>
@@ -85,6 +121,15 @@
     <t>(2.0322-22.3547j)</t>
   </si>
   <si>
+    <t>42954.9964j</t>
+  </si>
+  <si>
+    <t>477.2777j</t>
+  </si>
+  <si>
+    <t>238.6389j</t>
+  </si>
+  <si>
     <t>5-6</t>
   </si>
   <si>
@@ -97,6 +142,15 @@
     <t>(0.2459-3.9348j)</t>
   </si>
   <si>
+    <t>254996.7925j</t>
+  </si>
+  <si>
+    <t>2833.2977j</t>
+  </si>
+  <si>
+    <t>1416.6488j</t>
+  </si>
+  <si>
     <t>6-7</t>
   </si>
   <si>
@@ -109,6 +163,15 @@
     <t>(0.3219-5.1499j)</t>
   </si>
   <si>
+    <t>194829.01j</t>
+  </si>
+  <si>
+    <t>2164.7668j</t>
+  </si>
+  <si>
+    <t>1082.3834j</t>
+  </si>
+  <si>
     <t>7-8</t>
   </si>
   <si>
@@ -121,6 +184,15 @@
     <t>(0.3907-4.2005j)</t>
   </si>
   <si>
+    <t>135019.3691j</t>
+  </si>
+  <si>
+    <t>1500.2152j</t>
+  </si>
+  <si>
+    <t>750.1076j</t>
+  </si>
+  <si>
     <t>1-8</t>
   </si>
   <si>
@@ -133,6 +205,15 @@
     <t>(0.1824-1.9613j)</t>
   </si>
   <si>
+    <t>289171.0374j</t>
+  </si>
+  <si>
+    <t>3213.0115j</t>
+  </si>
+  <si>
+    <t>1606.5058j</t>
+  </si>
+  <si>
     <t>1-6</t>
   </si>
   <si>
@@ -143,6 +224,15 @@
   </si>
   <si>
     <t>(0.1654-1.7781j)</t>
+  </si>
+  <si>
+    <t>318962.7605j</t>
+  </si>
+  <si>
+    <t>3544.0307j</t>
+  </si>
+  <si>
+    <t>1772.0153j</t>
   </si>
 </sst>
 </file>
@@ -161,7 +251,6 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -506,21 +595,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="18.83203125" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" customWidth="1"/>
-    <col min="4" max="4" width="17.1640625" customWidth="1"/>
-    <col min="5" max="5" width="14.83203125" customWidth="1"/>
+    <col min="2" max="2" width="23.83203125" customWidth="1"/>
+    <col min="3" max="3" width="27" customWidth="1"/>
+    <col min="4" max="4" width="24.33203125" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" customWidth="1"/>
+    <col min="6" max="6" width="21.5" customWidth="1"/>
+    <col min="7" max="7" width="22.5" customWidth="1"/>
+    <col min="8" max="8" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -536,158 +628,248 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E2">
         <v>199</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="E3">
         <v>164</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="E4">
         <v>416</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="E5">
         <v>137</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="E6">
         <v>812</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="D7" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="E7">
         <v>620</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G7" t="s">
+        <v>48</v>
+      </c>
+      <c r="H7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="D8" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="E8">
         <v>430</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F8" t="s">
+        <v>54</v>
+      </c>
+      <c r="G8" t="s">
+        <v>55</v>
+      </c>
+      <c r="H8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="D9" t="s">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="E9">
         <v>920</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F9" t="s">
+        <v>61</v>
+      </c>
+      <c r="G9" t="s">
+        <v>62</v>
+      </c>
+      <c r="H9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>64</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>65</v>
       </c>
       <c r="C10" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="D10" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="E10">
         <v>1015</v>
+      </c>
+      <c r="F10" t="s">
+        <v>68</v>
+      </c>
+      <c r="G10" t="s">
+        <v>69</v>
+      </c>
+      <c r="H10" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pynta og fjerna drit
</commit_message>
<xml_diff>
--- a/linjeimpedanser.xlsx
+++ b/linjeimpedanser.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marku\Desktop\IELET2118---Prosjekt-Lastflytanalyse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EF187D2-5635-41D4-9E36-0140FEBEF64B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{092C9B3B-5552-4A78-A8FB-335DF4778350}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Base Case" sheetId="1" r:id="rId1"/>
@@ -294,6 +294,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -331,12 +332,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -644,19 +648,19 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="42.7109375" customWidth="1"/>
-    <col min="3" max="3" width="44.85546875" customWidth="1"/>
-    <col min="4" max="4" width="40.42578125" customWidth="1"/>
+    <col min="2" max="2" width="43.85546875" customWidth="1"/>
+    <col min="3" max="3" width="48.28515625" customWidth="1"/>
+    <col min="4" max="4" width="44.140625" customWidth="1"/>
     <col min="5" max="5" width="13.85546875" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" customWidth="1"/>
-    <col min="7" max="7" width="27.85546875" customWidth="1"/>
-    <col min="8" max="8" width="23.42578125" customWidth="1"/>
-    <col min="9" max="9" width="25.140625" customWidth="1"/>
+    <col min="6" max="6" width="24.85546875" customWidth="1"/>
+    <col min="7" max="7" width="30" customWidth="1"/>
+    <col min="8" max="8" width="25.5703125" customWidth="1"/>
+    <col min="9" max="9" width="27.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -692,28 +696,28 @@
       <c r="A2" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="3">
         <v>199.23</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="3" t="s">
         <v>15</v>
       </c>
     </row>
@@ -721,28 +725,28 @@
       <c r="A3" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="3">
         <v>163.56</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="3" t="s">
         <v>22</v>
       </c>
     </row>
@@ -750,28 +754,28 @@
       <c r="A4" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="3">
         <v>415.86</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="3" t="s">
         <v>29</v>
       </c>
     </row>
@@ -779,28 +783,28 @@
       <c r="A5" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="3">
         <v>136.72999999999999</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="3" t="s">
         <v>36</v>
       </c>
     </row>
@@ -808,28 +812,28 @@
       <c r="A6" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="3">
         <v>811.68000000000006</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="3" t="s">
         <v>43</v>
       </c>
     </row>
@@ -837,28 +841,28 @@
       <c r="A7" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="3">
         <v>620.16</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" s="3" t="s">
         <v>50</v>
       </c>
     </row>
@@ -866,28 +870,28 @@
       <c r="A8" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="3">
         <v>429.78</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" s="3" t="s">
         <v>57</v>
       </c>
     </row>
@@ -895,28 +899,28 @@
       <c r="A9" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="3">
         <v>920.45999999999992</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" s="3" t="s">
         <v>64</v>
       </c>
     </row>
@@ -924,28 +928,28 @@
       <c r="A10" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="3">
         <v>1015.29</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" s="3" t="s">
         <v>71</v>
       </c>
     </row>

</xml_diff>

<commit_message>
prøver å fikse før revert
</commit_message>
<xml_diff>
--- a/linjeimpedanser.xlsx
+++ b/linjeimpedanser.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marku\Desktop\IELET2118---Prosjekt-Lastflytanalyse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{092C9B3B-5552-4A78-A8FB-335DF4778350}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EF187D2-5635-41D4-9E36-0140FEBEF64B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Base Case" sheetId="1" r:id="rId1"/>
@@ -294,7 +294,6 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -332,15 +331,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -648,19 +644,19 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="43.85546875" customWidth="1"/>
-    <col min="3" max="3" width="48.28515625" customWidth="1"/>
-    <col min="4" max="4" width="44.140625" customWidth="1"/>
+    <col min="2" max="2" width="42.7109375" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" customWidth="1"/>
+    <col min="4" max="4" width="40.42578125" customWidth="1"/>
     <col min="5" max="5" width="13.85546875" customWidth="1"/>
-    <col min="6" max="6" width="24.85546875" customWidth="1"/>
-    <col min="7" max="7" width="30" customWidth="1"/>
-    <col min="8" max="8" width="25.5703125" customWidth="1"/>
-    <col min="9" max="9" width="27.5703125" customWidth="1"/>
+    <col min="6" max="6" width="22.7109375" customWidth="1"/>
+    <col min="7" max="7" width="27.85546875" customWidth="1"/>
+    <col min="8" max="8" width="23.42578125" customWidth="1"/>
+    <col min="9" max="9" width="25.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -696,28 +692,28 @@
       <c r="A2" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2">
         <v>199.23</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" t="s">
         <v>15</v>
       </c>
     </row>
@@ -725,28 +721,28 @@
       <c r="A3" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3">
         <v>163.56</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" t="s">
         <v>21</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" t="s">
         <v>22</v>
       </c>
     </row>
@@ -754,28 +750,28 @@
       <c r="A4" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4">
         <v>415.86</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" t="s">
         <v>28</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" t="s">
         <v>29</v>
       </c>
     </row>
@@ -783,28 +779,28 @@
       <c r="A5" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5">
         <v>136.72999999999999</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" t="s">
         <v>33</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" t="s">
         <v>34</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" t="s">
         <v>35</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="I5" t="s">
         <v>36</v>
       </c>
     </row>
@@ -812,28 +808,28 @@
       <c r="A6" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" t="s">
         <v>39</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6">
         <v>811.68000000000006</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" t="s">
         <v>40</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" t="s">
         <v>41</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" t="s">
         <v>42</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="I6" t="s">
         <v>43</v>
       </c>
     </row>
@@ -841,28 +837,28 @@
       <c r="A7" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" t="s">
         <v>45</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" t="s">
         <v>46</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7">
         <v>620.16</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" t="s">
         <v>47</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" t="s">
         <v>48</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" t="s">
         <v>49</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="I7" t="s">
         <v>50</v>
       </c>
     </row>
@@ -870,28 +866,28 @@
       <c r="A8" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" t="s">
         <v>51</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" t="s">
         <v>52</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" t="s">
         <v>53</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8">
         <v>429.78</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" t="s">
         <v>54</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" t="s">
         <v>55</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" t="s">
         <v>56</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="I8" t="s">
         <v>57</v>
       </c>
     </row>
@@ -899,28 +895,28 @@
       <c r="A9" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" t="s">
         <v>58</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" t="s">
         <v>59</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" t="s">
         <v>60</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9">
         <v>920.45999999999992</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" t="s">
         <v>61</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" t="s">
         <v>62</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="H9" t="s">
         <v>63</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="I9" t="s">
         <v>64</v>
       </c>
     </row>
@@ -928,28 +924,28 @@
       <c r="A10" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" t="s">
         <v>65</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" t="s">
         <v>66</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" t="s">
         <v>67</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10">
         <v>1015.29</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" t="s">
         <v>68</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" t="s">
         <v>69</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="H10" t="s">
         <v>70</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="I10" t="s">
         <v>71</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Revertet tilbake sånn at System_data er originalt før tweaking på oppgave 4, før jeg gjør tweak i 4d)
</commit_message>
<xml_diff>
--- a/linjeimpedanser.xlsx
+++ b/linjeimpedanser.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marku\Desktop\IELET2118---Prosjekt-Lastflytanalyse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{092C9B3B-5552-4A78-A8FB-335DF4778350}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EF187D2-5635-41D4-9E36-0140FEBEF64B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Base Case" sheetId="1" r:id="rId1"/>
@@ -294,7 +294,6 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -332,15 +331,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -648,19 +644,19 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="43.85546875" customWidth="1"/>
-    <col min="3" max="3" width="48.28515625" customWidth="1"/>
-    <col min="4" max="4" width="44.140625" customWidth="1"/>
+    <col min="2" max="2" width="42.7109375" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" customWidth="1"/>
+    <col min="4" max="4" width="40.42578125" customWidth="1"/>
     <col min="5" max="5" width="13.85546875" customWidth="1"/>
-    <col min="6" max="6" width="24.85546875" customWidth="1"/>
-    <col min="7" max="7" width="30" customWidth="1"/>
-    <col min="8" max="8" width="25.5703125" customWidth="1"/>
-    <col min="9" max="9" width="27.5703125" customWidth="1"/>
+    <col min="6" max="6" width="22.7109375" customWidth="1"/>
+    <col min="7" max="7" width="27.85546875" customWidth="1"/>
+    <col min="8" max="8" width="23.42578125" customWidth="1"/>
+    <col min="9" max="9" width="25.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -696,28 +692,28 @@
       <c r="A2" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2">
         <v>199.23</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" t="s">
         <v>15</v>
       </c>
     </row>
@@ -725,28 +721,28 @@
       <c r="A3" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3">
         <v>163.56</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" t="s">
         <v>21</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" t="s">
         <v>22</v>
       </c>
     </row>
@@ -754,28 +750,28 @@
       <c r="A4" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4">
         <v>415.86</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" t="s">
         <v>28</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" t="s">
         <v>29</v>
       </c>
     </row>
@@ -783,28 +779,28 @@
       <c r="A5" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5">
         <v>136.72999999999999</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" t="s">
         <v>33</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" t="s">
         <v>34</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" t="s">
         <v>35</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="I5" t="s">
         <v>36</v>
       </c>
     </row>
@@ -812,28 +808,28 @@
       <c r="A6" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" t="s">
         <v>39</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6">
         <v>811.68000000000006</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" t="s">
         <v>40</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" t="s">
         <v>41</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" t="s">
         <v>42</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="I6" t="s">
         <v>43</v>
       </c>
     </row>
@@ -841,28 +837,28 @@
       <c r="A7" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" t="s">
         <v>45</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" t="s">
         <v>46</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7">
         <v>620.16</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" t="s">
         <v>47</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" t="s">
         <v>48</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" t="s">
         <v>49</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="I7" t="s">
         <v>50</v>
       </c>
     </row>
@@ -870,28 +866,28 @@
       <c r="A8" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" t="s">
         <v>51</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" t="s">
         <v>52</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" t="s">
         <v>53</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8">
         <v>429.78</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" t="s">
         <v>54</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" t="s">
         <v>55</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" t="s">
         <v>56</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="I8" t="s">
         <v>57</v>
       </c>
     </row>
@@ -899,28 +895,28 @@
       <c r="A9" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" t="s">
         <v>58</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" t="s">
         <v>59</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" t="s">
         <v>60</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9">
         <v>920.45999999999992</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" t="s">
         <v>61</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" t="s">
         <v>62</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="H9" t="s">
         <v>63</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="I9" t="s">
         <v>64</v>
       </c>
     </row>
@@ -928,28 +924,28 @@
       <c r="A10" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" t="s">
         <v>65</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" t="s">
         <v>66</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" t="s">
         <v>67</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10">
         <v>1015.29</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" t="s">
         <v>68</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" t="s">
         <v>69</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="H10" t="s">
         <v>70</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="I10" t="s">
         <v>71</v>
       </c>
     </row>

</xml_diff>